<commit_message>
Selenium Version Changed 4.8.3
</commit_message>
<xml_diff>
--- a/Report-ScreenShot/ExcelReport/ExcelResult.xlsx
+++ b/Report-ScreenShot/ExcelReport/ExcelResult.xlsx
@@ -35,7 +35,7 @@
     <t>getUser</t>
   </si>
   <si>
-    <t>13:38:01.518341200</t>
+    <t>04:03:59.302590400</t>
   </si>
   <si>
     <t>testCase.demo1</t>
@@ -44,19 +44,19 @@
     <t>2</t>
   </si>
   <si>
-    <t>saucedemo1</t>
+    <t>saucedemo2</t>
   </si>
   <si>
-    <t>13:38:26.960488700</t>
+    <t>04:04:36.417331300</t>
   </si>
   <si>
     <t>3</t>
   </si>
   <si>
-    <t>saucedemo2</t>
+    <t>saucedemo1</t>
   </si>
   <si>
-    <t>13:38:42.612249600</t>
+    <t>04:04:36.986213500</t>
   </si>
 </sst>
 </file>

</xml_diff>